<commit_message>
remaking part 1 413
</commit_message>
<xml_diff>
--- a/TERM3/T3B2-ICTNPL413-Evaluate_net_regulations_legislation_telecommunications_industry/2-ICTNPL413-Assessment_Task 2/Assessmet-questions/tables.xlsx
+++ b/TERM3/T3B2-ICTNPL413-Evaluate_net_regulations_legislation_telecommunications_industry/2-ICTNPL413-Assessment_Task 2/Assessmet-questions/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\Assessments\TERM3\T3B2-ICTNPL413-Evaluate_net_regulations_legislation_telecommunications_industry\2-ICTNPL413-Assessment_Task 2\Assessmet-questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C1ED5C4-5B9A-4E74-AB7A-51708261070B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B418C5-FEB0-4407-A8C6-94D59DD60503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1776" yWindow="3360" windowWidth="19344" windowHeight="8880" xr2:uid="{73AC2B45-9F71-479A-BE50-0776A31F061D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73AC2B45-9F71-479A-BE50-0776A31F061D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,204 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t>3. Identify and summarise legislation relevant to the networking industry.</t>
+  </si>
+  <si>
+    <t>Competition and Consumer Act 2010</t>
+  </si>
+  <si>
+    <t>Broadcasting Services Act 1992</t>
+  </si>
+  <si>
+    <t>Radiocommunications Act 1992</t>
+  </si>
+  <si>
+    <t>Telecommunications (Consumer Protection and Service Standards) Act 1999</t>
+  </si>
+  <si>
+    <t>Privacy Act 1988</t>
+  </si>
+  <si>
+    <t>Telecommunications (Interception and Access) Act 1979</t>
+  </si>
+  <si>
+    <t>National Broadband Network Companies Act 2011</t>
+  </si>
+  <si>
+    <t>Telecommunications Act 1997</t>
+  </si>
+  <si>
+    <t>Australian Communications and Media Authority Act 2005</t>
+  </si>
+  <si>
+    <t>Online Safety Act 2021</t>
+  </si>
+  <si>
+    <t>Criminal Code Act 1995</t>
+  </si>
+  <si>
+    <t>Telecommunications and Other Legislation Amendment (Assistance and Access) Act 2018</t>
+  </si>
+  <si>
+    <t>Copyright Act 1968</t>
+  </si>
+  <si>
+    <t>Legislation</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A05145/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A00441/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A02124/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2011A00022/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2005A00044/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A00109/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A04401/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A04465/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A03712/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2021A00076/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2004A04868/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C2018A00148/latest</t>
+  </si>
+  <si>
+    <t>https://www.legislation.gov.au/C1968A00063/latest</t>
+  </si>
+  <si>
+    <t>Main functions</t>
+  </si>
+  <si>
+    <t>Establishes the regulatory framework for carriers and carriage service providers in Australia.</t>
+  </si>
+  <si>
+    <t>Defines obligations of telcos, licensing, consumer safeguards, and ACMA’s regulatory powers.</t>
+  </si>
+  <si>
+    <t>Provides minimum standards for consumer protection and universal service obligations.</t>
+  </si>
+  <si>
+    <t>Ensures access to basic phone services, customer service guarantees, funding for universal service.</t>
+  </si>
+  <si>
+    <t>Prohibits unauthorised interception of communications while allowing lawful access for enforcement and security.</t>
+  </si>
+  <si>
+    <t>Sets out interception warrants, stored communication access, and data retention obligations.</t>
+  </si>
+  <si>
+    <t>Creates the legislative framework for NBN Co operations.</t>
+  </si>
+  <si>
+    <t>Governs ownership, functions, reporting obligations, competition rules, and restrictions on private sector control.</t>
+  </si>
+  <si>
+    <t>Establishes the ACMA by merging previous agencies.</t>
+  </si>
+  <si>
+    <t>Regulates broadcasting, radiocommunications, telecommunications, online content, and enforces compliance.</t>
+  </si>
+  <si>
+    <t>Replaced the Trade Practices Act; sets competition rules and consumer protections.</t>
+  </si>
+  <si>
+    <t>Enforces anti-competitive conduct rules, merger control, consumer law, and regulates telco access arrangements.</t>
+  </si>
+  <si>
+    <t>Governs broadcasting, subscription television, and online media content.</t>
+  </si>
+  <si>
+    <t>Licences broadcasters, regulates Australian content, media diversity, advertising, and classification obligations.</t>
+  </si>
+  <si>
+    <t>Regulates use of the radiofrequency spectrum.</t>
+  </si>
+  <si>
+    <t>Spectrum licensing, interference management, technical standards, and ACMA’s enforcement powers.</t>
+  </si>
+  <si>
+    <t>Sets national privacy principles for handling personal information.</t>
+  </si>
+  <si>
+    <t>Governs data collection, storage, disclosure; creates OAIC as regulator; covers credit reporting and government records.</t>
+  </si>
+  <si>
+    <t>Strengthens powers of the eSafety Commissioner to tackle harmful online content.</t>
+  </si>
+  <si>
+    <t>Removal notices, restrictions on cyber-abuse, protection of children, enforcement against online service providers.</t>
+  </si>
+  <si>
+    <t>Consolidates federal criminal law, including computer and communication offences.</t>
+  </si>
+  <si>
+    <t>Defines terrorism, fraud, cybercrime, misuse of telecommunications services, and penalties.</t>
+  </si>
+  <si>
+    <t>Expands law-enforcement powers to access encrypted communications.</t>
+  </si>
+  <si>
+    <t>Compels providers to assist agencies, creates new warrant and technical capability powers, balances security with privacy concerns.</t>
+  </si>
+  <si>
+    <t>Main statute governing copyright in Australia.</t>
+  </si>
+  <si>
+    <t>Protects literary, musical, artistic works and broadcasts; sets exceptions, licensing schemes, and enforcement of rights.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,7 +246,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -62,14 +254,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,12 +696,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78CD9C8-13E6-4624-9BAA-B85DC828C760}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.77734375" customWidth="1"/>
+    <col min="3" max="3" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>